<commit_message>
The basic functionalities is now available in the UI.
</commit_message>
<xml_diff>
--- a/main_code/model.xlsx
+++ b/main_code/model.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>path</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>..\datasets\sample\y\wallhaven-5wgde9.png</t>
+  </si>
+  <si>
+    <t>C:\Users\rektplorer64\OneDrive\Pictures\Wallpapers\IMG_3037-scaled.jpg</t>
   </si>
 </sst>
 </file>
@@ -114,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -144,11 +147,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -172,6 +177,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -181,10 +188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N13"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="59" customWidth="true"/>
+    <col min="1" max="1" width="67.5703125" customWidth="true"/>
     <col min="2" max="2" width="5.28515625" customWidth="true"/>
     <col min="3" max="3" width="11.7109375" customWidth="true"/>
     <col min="4" max="4" width="11.7109375" customWidth="true"/>
@@ -264,7 +271,7 @@
         <v>218.68215263949918</v>
       </c>
       <c r="G2">
-        <v>2291.07125</v>
+        <v>3511.8525</v>
       </c>
       <c r="H2">
         <v>742.88639984550025</v>
@@ -282,10 +289,10 @@
         <v>76.265436324278497</v>
       </c>
       <c r="M2">
-        <v>40229.737500000003</v>
+        <v>43831.949999999997</v>
       </c>
       <c r="N2">
-        <v>51829.150000000001</v>
+        <v>55403.525000000001</v>
       </c>
     </row>
     <row r="3">
@@ -308,7 +315,7 @@
         <v>69.489700012207024</v>
       </c>
       <c r="G3">
-        <v>56747.092499999999</v>
+        <v>34492.970000000001</v>
       </c>
       <c r="H3">
         <v>129.00200164768813</v>
@@ -326,10 +333,10 @@
         <v>99.839620884622875</v>
       </c>
       <c r="M3">
-        <v>575.8125</v>
+        <v>609.47500000000002</v>
       </c>
       <c r="N3">
-        <v>690.07500000000005</v>
+        <v>706.96249999999998</v>
       </c>
     </row>
     <row r="4">
@@ -352,7 +359,7 @@
         <v>60.045857657967126</v>
       </c>
       <c r="G4">
-        <v>24879.220000000001</v>
+        <v>18967.341250000001</v>
       </c>
       <c r="H4">
         <v>158.39894777216981</v>
@@ -370,10 +377,10 @@
         <v>99.802693616046241</v>
       </c>
       <c r="M4">
-        <v>288.10000000000002</v>
+        <v>275.3125</v>
       </c>
       <c r="N4">
-        <v>343.35000000000002</v>
+        <v>312.53750000000002</v>
       </c>
     </row>
     <row r="5">
@@ -396,7 +403,7 @@
         <v>38.451444019274376</v>
       </c>
       <c r="G5">
-        <v>64670.527499999997</v>
+        <v>63839.386250000003</v>
       </c>
       <c r="H5">
         <v>436.44672557587097</v>
@@ -414,10 +421,10 @@
         <v>95.313449061275833</v>
       </c>
       <c r="M5">
-        <v>16442.900000000001</v>
+        <v>16886.900000000001</v>
       </c>
       <c r="N5">
-        <v>18508.325000000001</v>
+        <v>18954.924999999999</v>
       </c>
     </row>
     <row r="6">
@@ -440,7 +447,7 @@
         <v>49.30755185185172</v>
       </c>
       <c r="G6">
-        <v>71760.581250000003</v>
+        <v>37088.654999999999</v>
       </c>
       <c r="H6">
         <v>350.64597973925532</v>
@@ -458,10 +465,10 @@
         <v>97.971465847443767</v>
       </c>
       <c r="M6">
-        <v>1894.5999999999999</v>
+        <v>19110.849999999999</v>
       </c>
       <c r="N6">
-        <v>2205.9375</v>
+        <v>21103.337500000001</v>
       </c>
     </row>
     <row r="7">
@@ -484,7 +491,7 @@
         <v>39.382593858507036</v>
       </c>
       <c r="G7">
-        <v>34953.792500000003</v>
+        <v>32566.193749999999</v>
       </c>
       <c r="H7">
         <v>573.19277514401233</v>
@@ -502,10 +509,10 @@
         <v>92.765718300747864</v>
       </c>
       <c r="M7">
-        <v>5782.1999999999998</v>
+        <v>15017.6</v>
       </c>
       <c r="N7">
-        <v>6591.1875</v>
+        <v>15408.325000000001</v>
       </c>
     </row>
     <row r="8">
@@ -528,7 +535,7 @@
         <v>86.712397280092446</v>
       </c>
       <c r="G8">
-        <v>17216.16375</v>
+        <v>17404.142500000002</v>
       </c>
       <c r="H8">
         <v>519.78138623771531</v>
@@ -546,10 +553,10 @@
         <v>93.59475294856135</v>
       </c>
       <c r="M8">
-        <v>7706.0249999999996</v>
+        <v>7497.2749999999996</v>
       </c>
       <c r="N8">
-        <v>8503.8374999999996</v>
+        <v>8292.1499999999996</v>
       </c>
     </row>
     <row r="9">
@@ -572,7 +579,7 @@
         <v>73.404148341049307</v>
       </c>
       <c r="G9">
-        <v>16017.50625</v>
+        <v>15673.893749999999</v>
       </c>
       <c r="H9">
         <v>449.09417711155976</v>
@@ -590,10 +597,10 @@
         <v>95.324938159020604</v>
       </c>
       <c r="M9">
-        <v>1345.05</v>
+        <v>2407.625</v>
       </c>
       <c r="N9">
-        <v>1378.9375</v>
+        <v>2611.0999999999999</v>
       </c>
     </row>
     <row r="10">
@@ -616,7 +623,7 @@
         <v>78.812157118055524</v>
       </c>
       <c r="G10">
-        <v>20123.55875</v>
+        <v>20031.605</v>
       </c>
       <c r="H10">
         <v>469.28090819823166</v>
@@ -634,10 +641,10 @@
         <v>94.745899505364093</v>
       </c>
       <c r="M10">
-        <v>2636.2750000000001</v>
+        <v>2763.5250000000001</v>
       </c>
       <c r="N10">
-        <v>3088.6500000000001</v>
+        <v>3248.5875000000001</v>
       </c>
     </row>
     <row r="11">
@@ -660,7 +667,7 @@
         <v>132.58656394675918</v>
       </c>
       <c r="G11">
-        <v>7398.8575000000001</v>
+        <v>5611.2600000000002</v>
       </c>
       <c r="H11">
         <v>658.09302308018789</v>
@@ -678,10 +685,10 @@
         <v>85.1786732714625</v>
       </c>
       <c r="M11">
-        <v>18910.974999999999</v>
+        <v>15740.387500000001</v>
       </c>
       <c r="N11">
-        <v>21050.087500000001</v>
+        <v>17926.424999999999</v>
       </c>
     </row>
     <row r="12">
@@ -704,7 +711,7 @@
         <v>51.191011126192919</v>
       </c>
       <c r="G12">
-        <v>18998.720000000001</v>
+        <v>13268.577499999999</v>
       </c>
       <c r="H12">
         <v>528.59895652530304</v>
@@ -722,10 +729,54 @@
         <v>94.155926306730805</v>
       </c>
       <c r="M12">
-        <v>2260.7125000000001</v>
+        <v>13273.575000000001</v>
       </c>
       <c r="N12">
-        <v>2560.1999999999998</v>
+        <v>14464.9</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>78.605983529691486</v>
+      </c>
+      <c r="D13">
+        <v>45.935591121618785</v>
+      </c>
+      <c r="E13">
+        <v>84.152029070688855</v>
+      </c>
+      <c r="F13">
+        <v>60.045857657967126</v>
+      </c>
+      <c r="G13">
+        <v>18967.341250000001</v>
+      </c>
+      <c r="H13">
+        <v>158.39894777216981</v>
+      </c>
+      <c r="I13">
+        <v>254.20248607734547</v>
+      </c>
+      <c r="J13">
+        <v>0.39875475888324874</v>
+      </c>
+      <c r="K13">
+        <v>99.930153126919222</v>
+      </c>
+      <c r="L13">
+        <v>99.802693616046241</v>
+      </c>
+      <c r="M13">
+        <v>275.3125</v>
+      </c>
+      <c r="N13">
+        <v>312.53750000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added files required for the evaluation stage.
</commit_message>
<xml_diff>
--- a/main_code/model.xlsx
+++ b/main_code/model.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>path</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>..\datasets\sample\y\wallhaven-5wgde9.png</t>
-  </si>
-  <si>
-    <t>C:\Users\rektplorer64\OneDrive\Pictures\Wallpapers\IMG_3037-scaled.jpg</t>
   </si>
 </sst>
 </file>
@@ -117,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -147,13 +144,11 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -177,8 +172,6 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -188,10 +181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N12"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="67.5703125" customWidth="true"/>
+    <col min="1" max="1" width="59" customWidth="true"/>
     <col min="2" max="2" width="5.28515625" customWidth="true"/>
     <col min="3" max="3" width="11.7109375" customWidth="true"/>
     <col min="4" max="4" width="11.7109375" customWidth="true"/>
@@ -203,8 +196,8 @@
     <col min="10" max="10" width="12.7109375" customWidth="true"/>
     <col min="11" max="11" width="11.7109375" customWidth="true"/>
     <col min="12" max="12" width="13" customWidth="true"/>
-    <col min="13" max="13" width="10.7109375" customWidth="true"/>
-    <col min="14" max="14" width="10.7109375" customWidth="true"/>
+    <col min="13" max="13" width="13.7109375" customWidth="true"/>
+    <col min="14" max="14" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -271,10 +264,10 @@
         <v>218.68215263949918</v>
       </c>
       <c r="G2">
-        <v>3511.8525</v>
+        <v>201.40649230585709</v>
       </c>
       <c r="H2">
-        <v>742.88639984550025</v>
+        <v>7428.8639984550027</v>
       </c>
       <c r="I2">
         <v>386.12019151742334</v>
@@ -289,10 +282,10 @@
         <v>76.265436324278497</v>
       </c>
       <c r="M2">
-        <v>43831.949999999997</v>
+        <v>25.137841923673367</v>
       </c>
       <c r="N2">
-        <v>55403.525000000001</v>
+        <v>31.7741978959249</v>
       </c>
     </row>
     <row r="3">
@@ -315,10 +308,10 @@
         <v>69.489700012207024</v>
       </c>
       <c r="G3">
-        <v>34492.970000000001</v>
+        <v>526.32095336914063</v>
       </c>
       <c r="H3">
-        <v>129.00200164768813</v>
+        <v>1290.0200164768814</v>
       </c>
       <c r="I3">
         <v>199.42995729704197</v>
@@ -333,10 +326,10 @@
         <v>99.839620884622875</v>
       </c>
       <c r="M3">
-        <v>609.47500000000002</v>
+        <v>0.092998504638671875</v>
       </c>
       <c r="N3">
-        <v>706.96249999999998</v>
+        <v>0.10787391662597655</v>
       </c>
     </row>
     <row r="4">
@@ -359,10 +352,10 @@
         <v>60.045857657967126</v>
       </c>
       <c r="G4">
-        <v>18967.341250000001</v>
+        <v>626.29904275412082</v>
       </c>
       <c r="H4">
-        <v>158.39894777216981</v>
+        <v>1583.989477721698</v>
       </c>
       <c r="I4">
         <v>254.20248607734547</v>
@@ -377,10 +370,10 @@
         <v>99.802693616046241</v>
       </c>
       <c r="M4">
-        <v>275.3125</v>
+        <v>0.090907815141589188</v>
       </c>
       <c r="N4">
-        <v>312.53750000000002</v>
+        <v>0.10319945979501269</v>
       </c>
     </row>
     <row r="5">
@@ -403,10 +396,10 @@
         <v>38.451444019274376</v>
       </c>
       <c r="G5">
-        <v>63839.386250000003</v>
+        <v>904.75320649092976</v>
       </c>
       <c r="H5">
-        <v>436.44672557587097</v>
+        <v>4364.4672557587101</v>
       </c>
       <c r="I5">
         <v>570.84544570999788</v>
@@ -421,10 +414,10 @@
         <v>95.313449061275833</v>
       </c>
       <c r="M5">
-        <v>16886.900000000001</v>
+        <v>2.3932681405895697</v>
       </c>
       <c r="N5">
-        <v>18954.924999999999</v>
+        <v>2.6863555839002267</v>
       </c>
     </row>
     <row r="6">
@@ -447,10 +440,10 @@
         <v>49.30755185185172</v>
       </c>
       <c r="G6">
-        <v>37088.654999999999</v>
+        <v>508.76069958847734</v>
       </c>
       <c r="H6">
-        <v>350.64597973925532</v>
+        <v>3506.4597973925534</v>
       </c>
       <c r="I6">
         <v>402.32254598512446</v>
@@ -465,10 +458,10 @@
         <v>97.971465847443767</v>
       </c>
       <c r="M6">
-        <v>19110.849999999999</v>
+        <v>2.6215157750342932</v>
       </c>
       <c r="N6">
-        <v>21103.337500000001</v>
+        <v>2.8948336762688616</v>
       </c>
     </row>
     <row r="7">
@@ -491,10 +484,10 @@
         <v>39.382593858507036</v>
       </c>
       <c r="G7">
-        <v>32566.193749999999</v>
+        <v>883.41454399956604</v>
       </c>
       <c r="H7">
-        <v>573.19277514401233</v>
+        <v>5731.9277514401228</v>
       </c>
       <c r="I7">
         <v>350.00763056356141</v>
@@ -509,10 +502,10 @@
         <v>92.765718300747864</v>
       </c>
       <c r="M7">
-        <v>15017.6</v>
+        <v>4.0737847222222223</v>
       </c>
       <c r="N7">
-        <v>15408.325000000001</v>
+        <v>4.1797756618923616</v>
       </c>
     </row>
     <row r="8">
@@ -535,10 +528,10 @@
         <v>86.712397280092446</v>
       </c>
       <c r="G8">
-        <v>17404.142500000002</v>
+        <v>839.32014371141975</v>
       </c>
       <c r="H8">
-        <v>519.78138623771531</v>
+        <v>5197.8138623771529</v>
       </c>
       <c r="I8">
         <v>293.29793561439294</v>
@@ -553,10 +546,10 @@
         <v>93.59475294856135</v>
       </c>
       <c r="M8">
-        <v>7497.2749999999996</v>
+        <v>3.6155840084876538</v>
       </c>
       <c r="N8">
-        <v>8292.1499999999996</v>
+        <v>3.9989149305555554</v>
       </c>
     </row>
     <row r="9">
@@ -579,10 +572,10 @@
         <v>73.404148341049307</v>
       </c>
       <c r="G9">
-        <v>15673.893749999999</v>
+        <v>755.87836371527771</v>
       </c>
       <c r="H9">
-        <v>449.09417711155976</v>
+        <v>4490.9417711155975</v>
       </c>
       <c r="I9">
         <v>194.45358572214704</v>
@@ -597,10 +590,10 @@
         <v>95.324938159020604</v>
       </c>
       <c r="M9">
-        <v>2407.625</v>
+        <v>1.161084587191358</v>
       </c>
       <c r="N9">
-        <v>2611.0999999999999</v>
+        <v>1.2592110339506171</v>
       </c>
     </row>
     <row r="10">
@@ -623,10 +616,10 @@
         <v>78.812157118055524</v>
       </c>
       <c r="G10">
-        <v>20031.605</v>
+        <v>869.42730034722229</v>
       </c>
       <c r="H10">
-        <v>469.28090819823166</v>
+        <v>4692.8090819823165</v>
       </c>
       <c r="I10">
         <v>226.53651269833392</v>
@@ -641,10 +634,10 @@
         <v>94.745899505364093</v>
       </c>
       <c r="M10">
-        <v>2763.5250000000001</v>
+        <v>1.1994466145833333</v>
       </c>
       <c r="N10">
-        <v>3248.5875000000001</v>
+        <v>1.4099772135416668</v>
       </c>
     </row>
     <row r="11">
@@ -667,10 +660,10 @@
         <v>132.58656394675918</v>
       </c>
       <c r="G11">
-        <v>5611.2600000000002</v>
+        <v>270.60474537037038</v>
       </c>
       <c r="H11">
-        <v>658.09302308018789</v>
+        <v>6580.9302308018796</v>
       </c>
       <c r="I11">
         <v>141.38159496193626</v>
@@ -685,10 +678,10 @@
         <v>85.1786732714625</v>
       </c>
       <c r="M11">
-        <v>15740.387500000001</v>
+        <v>7.590850453317902</v>
       </c>
       <c r="N11">
-        <v>17926.424999999999</v>
+        <v>8.6450737847222232</v>
       </c>
     </row>
     <row r="12">
@@ -711,10 +704,10 @@
         <v>51.191011126192919</v>
       </c>
       <c r="G12">
-        <v>13268.577499999999</v>
+        <v>682.20310443402434</v>
       </c>
       <c r="H12">
-        <v>528.59895652530304</v>
+        <v>5285.9895652530304</v>
       </c>
       <c r="I12">
         <v>248.07260875983707</v>
@@ -729,54 +722,10 @@
         <v>94.155926306730805</v>
       </c>
       <c r="M12">
-        <v>13273.575000000001</v>
+        <v>6.8246005059230015</v>
       </c>
       <c r="N12">
-        <v>14464.9</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>78.605983529691486</v>
-      </c>
-      <c r="D13">
-        <v>45.935591121618785</v>
-      </c>
-      <c r="E13">
-        <v>84.152029070688855</v>
-      </c>
-      <c r="F13">
-        <v>60.045857657967126</v>
-      </c>
-      <c r="G13">
-        <v>18967.341250000001</v>
-      </c>
-      <c r="H13">
-        <v>158.39894777216981</v>
-      </c>
-      <c r="I13">
-        <v>254.20248607734547</v>
-      </c>
-      <c r="J13">
-        <v>0.39875475888324874</v>
-      </c>
-      <c r="K13">
-        <v>99.930153126919222</v>
-      </c>
-      <c r="L13">
-        <v>99.802693616046241</v>
-      </c>
-      <c r="M13">
-        <v>275.3125</v>
-      </c>
-      <c r="N13">
-        <v>312.53750000000002</v>
+        <v>7.4371195294504773</v>
       </c>
     </row>
   </sheetData>

</xml_diff>